<commit_message>
Update fuel calcs spreadsheet
</commit_message>
<xml_diff>
--- a/assets/fuel-calcs.xlsx
+++ b/assets/fuel-calcs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewminer/Twitch/Minecraft/Instances/brunel-3/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF4FCDA-AD55-FE4B-8056-046DBE1E8528}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30BA247B-8930-CD41-B7C7-0E870950AD8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8540" yWindow="460" windowWidth="34140" windowHeight="28340" activeTab="4" xr2:uid="{7AE51FE2-D37D-804E-BEE6-C97F5A6C5473}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="28340" activeTab="6" xr2:uid="{7AE51FE2-D37D-804E-BEE6-C97F5A6C5473}"/>
   </bookViews>
   <sheets>
     <sheet name="worksheet" sheetId="1" r:id="rId1"/>
@@ -6163,8 +6163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3E01491-3967-D748-BDE4-30FCB604639B}">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -8369,7 +8369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93638DD5-F4B4-1C48-94A9-5CE13A38D571}">
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updates for new server
</commit_message>
<xml_diff>
--- a/assets/fuel-calcs.xlsx
+++ b/assets/fuel-calcs.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewminer/Twitch/Minecraft/Instances/brunel-3/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewminer/Documents/curseforge/minecraft/Instances/brunel-3/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD270452-D883-5748-9480-438CA12CD5D3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57599D76-53BE-494D-97CA-57431953A1B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="28340" activeTab="1" xr2:uid="{7AE51FE2-D37D-804E-BEE6-C97F5A6C5473}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{7AE51FE2-D37D-804E-BEE6-C97F5A6C5473}"/>
   </bookViews>
   <sheets>
     <sheet name="worksheet" sheetId="1" r:id="rId1"/>
     <sheet name="results" sheetId="16" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" refMode="R1C1"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="55">
   <si>
     <t>biodiesel</t>
   </si>
@@ -175,12 +176,6 @@
     <t>portable generator</t>
   </si>
   <si>
-    <t>pumpjack (full)</t>
-  </si>
-  <si>
-    <t>pumpjack (residual)</t>
-  </si>
-  <si>
     <t>diesel excess gas.</t>
   </si>
   <si>
@@ -203,6 +198,9 @@
   </si>
   <si>
     <t>Diesel + Gasoline (full)</t>
+  </si>
+  <si>
+    <t>pumpjack</t>
   </si>
 </sst>
 </file>
@@ -571,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB7D62C-4FBD-C147-A71B-DF9E27B49908}">
-  <dimension ref="A1:M48"/>
+  <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -632,63 +630,63 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1">
+        <f>2*E35</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="4">
+        <v>1024</v>
+      </c>
+      <c r="L2" s="1">
+        <f t="shared" ref="L2:L36" si="0">B2*K2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3">
-        <f>SUMIF(D:D, A2, E:E)</f>
-        <v>0</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" s="3">
+        <f>SUMIF(D:D, A3, E:E)</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="3">
-        <f>100/90*B2</f>
-        <v>0</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="E3" s="3">
+        <f>100/90*B3</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K3" s="4">
         <f>12500/90</f>
         <v>138.88888888888889</v>
       </c>
-      <c r="L2" s="1">
-        <f>B2*K2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="3">
-        <f>SUMIF(D:D, A3, E:E)</f>
-        <v>0</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K3" s="4">
-        <v>10240</v>
-      </c>
       <c r="L3" s="1">
-        <f t="shared" ref="L3:L35" si="0">B3*K3</f>
+        <f>B3*K3</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="3">
-        <f>SUMIF(F:F, A4, G:G)</f>
+        <f>SUMIF(D:D, A4, E:E)</f>
         <v>0</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>41</v>
       </c>
       <c r="K4" s="4">
-        <v>8192</v>
+        <v>10240</v>
       </c>
       <c r="L4" s="1">
         <f t="shared" si="0"/>
@@ -697,17 +695,17 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B5" s="3">
-        <f>SUMIF(D:D, A5, E:E)</f>
+        <f>SUMIF(F:F, A5, G:G)</f>
         <v>0</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>41</v>
       </c>
       <c r="K5" s="4">
-        <v>4096</v>
+        <v>8192</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" si="0"/>
@@ -716,7 +714,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B6" s="3">
         <f>SUMIF(D:D, A6, E:E)</f>
@@ -726,7 +724,7 @@
         <v>41</v>
       </c>
       <c r="K6" s="4">
-        <v>1024</v>
+        <v>4096</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="0"/>
@@ -735,17 +733,17 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="3">
-        <f>SUMIF(F:F, A7, G:G)</f>
+        <f>SUMIF(D:D, A7, E:E)</f>
         <v>0</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>41</v>
       </c>
       <c r="K7" s="4">
-        <v>10240</v>
+        <v>256</v>
       </c>
       <c r="L7" s="1">
         <f t="shared" si="0"/>
@@ -754,17 +752,17 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B8" s="3">
-        <f>SUMIF(D:D, A8, E:E)</f>
+        <f>SUMIF(F:F, A8, G:G)</f>
         <v>0</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>41</v>
       </c>
       <c r="K8" s="4">
-        <v>1024</v>
+        <v>10240</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="0"/>
@@ -773,7 +771,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="3">
         <f>SUMIF(D:D, A9, E:E)</f>
@@ -792,92 +790,80 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B10" s="3">
-        <f>SUMIF(H:H, A10, I:I)</f>
-        <v>0</v>
+        <f>SUMIF(D:D, A10, E:E)</f>
+        <v>488.28125</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>41</v>
       </c>
       <c r="K10" s="4">
-        <v>0.25</v>
+        <v>512</v>
       </c>
       <c r="L10" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>250000</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B11" s="3">
-        <f>SUMIF(D:D, A11, E:E)</f>
-        <v>1953.125</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="3">
-        <f>100/40*B11</f>
-        <v>4882.8125</v>
+        <f>SUMIF(H:H, A11, I:I)</f>
+        <v>0</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="K11" s="4">
-        <f>1024/40</f>
-        <v>25.6</v>
+        <v>0.25</v>
       </c>
       <c r="L11" s="1">
         <f t="shared" si="0"/>
-        <v>50000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>2</v>
       </c>
       <c r="B12" s="3">
-        <f>B11/40*45</f>
-        <v>2197.265625</v>
+        <f>SUMIF(D:D, A12, E:E)</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3">
+        <f>1000/400*B12</f>
+        <v>0</v>
       </c>
       <c r="J12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K12" s="4">
+        <v>115.2</v>
+      </c>
+      <c r="L12" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="J13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K13" s="4">
         <f>-(256/5)</f>
         <v>-51.2</v>
       </c>
-      <c r="L12" s="1">
-        <f t="shared" si="0"/>
-        <v>-112500</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="3">
-        <f>SUMIF(F:F, A13, G:G)</f>
-        <v>0</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="3">
-        <f>100/30*B13</f>
-        <v>0</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K13" s="4">
-        <f>1024/30</f>
-        <v>34.133333333333333</v>
-      </c>
       <c r="L13" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -885,25 +871,24 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B14" s="3">
-        <f>SUMIF(D:D, A14, E:E)</f>
+        <f>SUMIF(F:F, A14, G:G)</f>
         <v>0</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E14" s="3">
-        <f>100/45*B14</f>
+        <f>1000/800*B14</f>
         <v>0</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>31</v>
       </c>
       <c r="K14" s="4">
-        <f>1024/45</f>
-        <v>22.755555555555556</v>
+        <v>57.6</v>
       </c>
       <c r="L14" s="1">
         <f t="shared" si="0"/>
@@ -912,25 +897,24 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="B15" s="3">
-        <f>SUMIF(F:F, A15, G:G)</f>
+        <f>SUMIF(D:D, A15, E:E)</f>
         <v>0</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="E15" s="3">
-        <f>8/640*B15</f>
+        <f>100/45*B15</f>
         <v>0</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K15" s="4">
-        <f>5120/640</f>
-        <v>8</v>
+        <v>115.2</v>
       </c>
       <c r="L15" s="1">
         <f t="shared" si="0"/>
@@ -939,40 +923,28 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="3"/>
+        <v>29</v>
+      </c>
+      <c r="B16" s="3">
+        <f>SUMIF(F:F, A16, G:G)</f>
+        <v>976.5625</v>
+      </c>
       <c r="D16" s="1" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="E16" s="3">
-        <f>20/1500*B16</f>
-        <v>0</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="4">
-        <f t="shared" ref="G16:G27" si="1">1/1500*B16</f>
-        <v>0</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I16" s="3">
-        <f t="shared" ref="I16:I27" si="2">1000/1500*B16</f>
-        <v>0</v>
+        <f>1/2*B16</f>
+        <v>488.28125</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="K16" s="4">
-        <f t="shared" ref="K16:K27" si="3">4096/1500</f>
-        <v>2.7306666666666666</v>
+        <v>128</v>
       </c>
       <c r="L16" s="1">
-        <f>B16*K16</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>125000</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -984,28 +956,28 @@
         <v>19</v>
       </c>
       <c r="E17" s="3">
-        <f>20/1500*B17</f>
+        <f>20/2000*B17</f>
         <v>0</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G17" s="4">
-        <f>1/1500*B17</f>
+        <f>1/2000*B17</f>
         <v>0</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="I17" s="3">
-        <f>1000/1500*B17</f>
+        <f>1000/2000*B17</f>
         <v>0</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K17" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="K17:K28" si="1">4096/1500</f>
         <v>2.7306666666666666</v>
       </c>
       <c r="L17" s="1">
@@ -1019,31 +991,31 @@
       </c>
       <c r="B18" s="3"/>
       <c r="D18" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E18" s="3">
-        <f>5/1500*B18</f>
+        <f>20/2000*B18</f>
         <v>0</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G18" s="4">
-        <f>1/1500*B18</f>
+        <f>1/2000*B18</f>
         <v>0</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="I18" s="3">
-        <f>1000/1500*B18</f>
+        <f>1000/2000*B18</f>
         <v>0</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K18" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>2.7306666666666666</v>
       </c>
       <c r="L18" s="1">
@@ -1060,32 +1032,32 @@
         <v>23</v>
       </c>
       <c r="E19" s="3">
-        <f>5/1500*B19</f>
+        <f>5/2000*B19</f>
         <v>0</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G19" s="4">
-        <f t="shared" si="1"/>
+        <f>1/2000*B19</f>
         <v>0</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="I19" s="3">
-        <f t="shared" si="2"/>
+        <f>1000/2000*B19</f>
         <v>0</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K19" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>2.7306666666666666</v>
       </c>
       <c r="L19" s="1">
-        <f t="shared" si="0"/>
+        <f>B19*K19</f>
         <v>0</v>
       </c>
     </row>
@@ -1095,31 +1067,31 @@
       </c>
       <c r="B20" s="3"/>
       <c r="D20" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E20" s="3">
-        <f>16/1500*B20</f>
+        <f>5/2000*B20</f>
         <v>0</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G20" s="4">
-        <f t="shared" si="1"/>
+        <f>1/2000*B20</f>
         <v>0</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="I20" s="3">
-        <f t="shared" si="2"/>
+        <f>1000/2000*B20</f>
         <v>0</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K20" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>2.7306666666666666</v>
       </c>
       <c r="L20" s="1">
@@ -1136,28 +1108,28 @@
         <v>19</v>
       </c>
       <c r="E21" s="3">
-        <f>16/1500*B21</f>
+        <f>16/2000*B21</f>
         <v>0</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G21" s="4">
-        <f t="shared" si="1"/>
+        <f>1/2000*B21</f>
         <v>0</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="I21" s="3">
-        <f t="shared" si="2"/>
+        <f>1000/2000*B21</f>
         <v>0</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K21" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>2.7306666666666666</v>
       </c>
       <c r="L21" s="1">
@@ -1169,33 +1141,36 @@
       <c r="A22" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="3"/>
+      <c r="B22" s="3">
+        <f>E14</f>
+        <v>0</v>
+      </c>
       <c r="D22" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E22" s="3">
-        <f>4/1500*B22</f>
+        <f>16/2000*B22</f>
         <v>0</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G22" s="4">
-        <f t="shared" si="1"/>
+        <f>1/2000*B22</f>
         <v>0</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="I22" s="3">
-        <f t="shared" si="2"/>
+        <f>1000/2000*B22</f>
         <v>0</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K22" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>2.7306666666666666</v>
       </c>
       <c r="L22" s="1">
@@ -1212,32 +1187,32 @@
         <v>23</v>
       </c>
       <c r="E23" s="3">
-        <f>4/1500*B23</f>
+        <f>4/2000*B23</f>
         <v>0</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G23" s="4">
-        <f t="shared" si="1"/>
+        <f>1/2000*B23</f>
         <v>0</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="I23" s="3">
-        <f t="shared" si="2"/>
+        <f>1000/2000*B23</f>
         <v>0</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K23" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>2.7306666666666666</v>
       </c>
       <c r="L23" s="1">
-        <f>B23*K23</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1247,35 +1222,35 @@
       </c>
       <c r="B24" s="3"/>
       <c r="D24" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E24" s="3">
-        <f>40/1500*B24</f>
+        <f>4/2000*B24</f>
         <v>0</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G24" s="4">
-        <f t="shared" si="1"/>
+        <f>1/2000*B24</f>
         <v>0</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I24" s="3">
-        <f t="shared" si="2"/>
+        <f>1000/2000*B24</f>
         <v>0</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K24" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>2.7306666666666666</v>
       </c>
       <c r="L24" s="1">
-        <f t="shared" si="0"/>
+        <f>B24*K24</f>
         <v>0</v>
       </c>
     </row>
@@ -1285,31 +1260,31 @@
       </c>
       <c r="B25" s="3"/>
       <c r="D25" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E25" s="3">
-        <f>10/1500*B25</f>
+        <f>40/2000*B25</f>
         <v>0</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G25" s="4">
-        <f t="shared" si="1"/>
+        <f>1/2000*B25</f>
         <v>0</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>25</v>
       </c>
       <c r="I25" s="3">
-        <f t="shared" si="2"/>
+        <f>1000/2000*B25</f>
         <v>0</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K25" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>2.7306666666666666</v>
       </c>
       <c r="L25" s="1">
@@ -1323,31 +1298,31 @@
       </c>
       <c r="B26" s="3"/>
       <c r="D26" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E26" s="3">
-        <f>32/1500*B26</f>
+        <f>10/2000*B26</f>
         <v>0</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G26" s="4">
-        <f t="shared" si="1"/>
+        <f>1/2000*B26</f>
         <v>0</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>25</v>
       </c>
       <c r="I26" s="3">
-        <f t="shared" si="2"/>
+        <f>1000/2000*B26</f>
         <v>0</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K26" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>2.7306666666666666</v>
       </c>
       <c r="L26" s="1">
@@ -1361,31 +1336,31 @@
       </c>
       <c r="B27" s="3"/>
       <c r="D27" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E27" s="3">
-        <f>8/1500*B27</f>
+        <f>32/2000*B27</f>
         <v>0</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G27" s="4">
-        <f t="shared" si="1"/>
+        <f>1/2000*B27</f>
         <v>0</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>25</v>
       </c>
       <c r="I27" s="3">
-        <f t="shared" si="2"/>
+        <f>1000/2000*B27</f>
         <v>0</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K27" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>2.7306666666666666</v>
       </c>
       <c r="L27" s="1">
@@ -1395,15 +1370,36 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B28" s="3"/>
+      <c r="D28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" s="3">
+        <f>8/2000*B28</f>
+        <v>0</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G28" s="4">
+        <f>1/2000*B28</f>
+        <v>0</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I28" s="3">
+        <f>1000/2000*B28</f>
+        <v>0</v>
+      </c>
       <c r="J28" s="1" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="K28" s="4">
-        <f>1024/6</f>
-        <v>170.66666666666666</v>
+        <f t="shared" si="1"/>
+        <v>2.7306666666666666</v>
       </c>
       <c r="L28" s="1">
         <f t="shared" si="0"/>
@@ -1412,134 +1408,124 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B29" s="3">
-        <f>E11</f>
-        <v>4882.8125</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B29" s="3"/>
       <c r="J29" s="1" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="K29" s="4">
-        <f>1024/15</f>
-        <v>68.266666666666666</v>
+        <v>6.4</v>
       </c>
       <c r="L29" s="1">
         <f t="shared" si="0"/>
-        <v>333333.33333333331</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B30" s="3"/>
-      <c r="D30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="3">
+        <f>E12</f>
+        <v>0</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K30" s="4">
+        <v>6.4</v>
+      </c>
+      <c r="L30" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="D31" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E30" s="3">
-        <f>50/100*B30</f>
-        <v>0</v>
-      </c>
-      <c r="F30" s="1" t="s">
+      <c r="E31" s="3">
+        <f>5/10*B31</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G30" s="4">
-        <f>50/100*B30</f>
-        <v>0</v>
-      </c>
-      <c r="J30" s="1" t="s">
+      <c r="G31" s="4">
+        <f>5/10*B31</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K30" s="4">
+      <c r="K31" s="4">
+        <v>6.4</v>
+      </c>
+      <c r="L31" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="3">
+        <f>E38</f>
+        <v>1953.125</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="3">
+        <f>50/100*B32</f>
+        <v>976.5625</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G32" s="4">
+        <f>50/100*B32</f>
+        <v>976.5625</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K32" s="4">
         <f>500/100</f>
         <v>5</v>
       </c>
-      <c r="L30" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31" s="3">
-        <f>E37</f>
-        <v>0</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" s="3">
-        <f>50/100*B31</f>
-        <v>0</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G31" s="4">
-        <f>50/100*B31</f>
-        <v>0</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K31" s="4">
-        <f>500/100</f>
-        <v>5</v>
-      </c>
-      <c r="L31" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+      <c r="L32" s="1">
+        <f t="shared" si="0"/>
+        <v>9765.625</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="3">
-        <f>SUMIF(H:H,A32,I:I)</f>
-        <v>0</v>
-      </c>
-      <c r="D32" s="1" t="s">
+      <c r="B33" s="3">
+        <f>SUMIF(H:H,A33,I:I)</f>
+        <v>0</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E32" s="3">
-        <f>20/2000*B32</f>
-        <v>0</v>
-      </c>
-      <c r="J32" s="1" t="s">
+      <c r="E33" s="3">
+        <f>20/2000*B33</f>
+        <v>0</v>
+      </c>
+      <c r="J33" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K32" s="4">
+      <c r="K33" s="4">
         <f>51200/2000</f>
         <v>25.6</v>
-      </c>
-      <c r="L32" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" s="3"/>
-      <c r="D33" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E33" s="3">
-        <f>20/4000*B33</f>
-        <v>0</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K33" s="4">
-        <f>64000/4000</f>
-        <v>16</v>
       </c>
       <c r="L33" s="1">
         <f t="shared" si="0"/>
@@ -1552,18 +1538,17 @@
       </c>
       <c r="B34" s="3"/>
       <c r="D34" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E34" s="3">
-        <f>1/350*B34</f>
+        <f>1/16*B34</f>
         <v>0</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>14</v>
       </c>
       <c r="K34" s="4">
-        <f>256/350</f>
-        <v>0.73142857142857143</v>
+        <v>64</v>
       </c>
       <c r="L34" s="1">
         <f t="shared" si="0"/>
@@ -1572,44 +1557,54 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B35" s="3">
-        <f>SUMIF(D:D, A35, E:E)</f>
+        <f>I22</f>
         <v>0</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E35" s="3">
-        <f>8/512*B35</f>
+        <f>1/32*B35</f>
         <v>0</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>14</v>
       </c>
       <c r="K35" s="4">
-        <f>51200/512</f>
-        <v>100</v>
+        <v>16</v>
       </c>
       <c r="L35" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E37" s="3">
-        <f>1000/512000*B37</f>
-        <v>0</v>
-      </c>
-      <c r="J37" s="1" t="s">
-        <v>36</v>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="3">
+        <f>E31</f>
+        <v>0</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" s="3">
+        <f>1/16*B36</f>
+        <v>0</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K36" s="4">
+        <v>64</v>
+      </c>
+      <c r="L36" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
@@ -1620,7 +1615,7 @@
         <v>1000000</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E38" s="3">
         <f>1000/512000*B38</f>
@@ -1635,56 +1630,71 @@
         <v>35</v>
       </c>
       <c r="D39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E39" s="3">
+        <f>1000/640000*B39</f>
+        <v>0</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E39" s="3">
-        <f>5/256*B39</f>
-        <v>0</v>
-      </c>
-      <c r="J39" s="1" t="s">
+      <c r="E40" s="3">
+        <f>5/256*B40</f>
+        <v>0</v>
+      </c>
+      <c r="J40" s="1" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B45" s="1">
-        <f>SUM(B37:B39)</f>
-        <v>1000000</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B46" s="1">
-        <f>SUM(L:L)</f>
-        <v>270833.33333333331</v>
+        <f>SUM(B38:B40)</f>
+        <v>1000000</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B47" s="1">
-        <f>B45-B46</f>
-        <v>729166.66666666674</v>
+        <f>SUM(L:L)</f>
+        <v>384765.625</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B48" s="1">
+        <f>B46-B47</f>
+        <v>615234.375</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B48" s="2">
-        <f>B47/B45</f>
-        <v>0.72916666666666674</v>
+      <c r="B49" s="2">
+        <f>B48/B46</f>
+        <v>0.615234375</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M35">
-    <sortCondition ref="J2:J35"/>
-    <sortCondition ref="A2:A35"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:M36">
+    <sortCondition ref="J3:J36"/>
+    <sortCondition ref="A3:A36"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1694,7 +1704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB5E60D2-D857-7D42-B91A-1C15BBBDB9B7}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -1705,37 +1715,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix issues discovered during game play
</commit_message>
<xml_diff>
--- a/assets/fuel-calcs.xlsx
+++ b/assets/fuel-calcs.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewminer/Documents/curseforge/minecraft/Instances/brunel-3/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewminer/Twitch/Minecraft/Instances/brunel-3/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57599D76-53BE-494D-97CA-57431953A1B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E705F7-E7D2-B544-A184-C043CE5DCA90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{7AE51FE2-D37D-804E-BEE6-C97F5A6C5473}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27420" windowHeight="25640" xr2:uid="{7AE51FE2-D37D-804E-BEE6-C97F5A6C5473}"/>
   </bookViews>
   <sheets>
     <sheet name="worksheet" sheetId="1" r:id="rId1"/>
     <sheet name="results" sheetId="16" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" refMode="R1C1"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -571,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB7D62C-4FBD-C147-A71B-DF9E27B49908}">
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -794,7 +793,7 @@
       </c>
       <c r="B10" s="3">
         <f>SUMIF(D:D, A10, E:E)</f>
-        <v>488.28125</v>
+        <v>0</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>41</v>
@@ -804,7 +803,7 @@
       </c>
       <c r="L10" s="1">
         <f t="shared" si="0"/>
-        <v>250000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -832,14 +831,14 @@
       </c>
       <c r="B12" s="3">
         <f>SUMIF(D:D, A12, E:E)</f>
-        <v>0</v>
+        <v>1562.5</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E12" s="3">
         <f>1000/400*B12</f>
-        <v>0</v>
+        <v>3906.25</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>31</v>
@@ -849,7 +848,7 @@
       </c>
       <c r="L12" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>180000</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -927,14 +926,14 @@
       </c>
       <c r="B16" s="3">
         <f>SUMIF(F:F, A16, G:G)</f>
-        <v>976.5625</v>
+        <v>0</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E16" s="3">
         <f>1/2*B16</f>
-        <v>488.28125</v>
+        <v>0</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>30</v>
@@ -944,7 +943,7 @@
       </c>
       <c r="L16" s="1">
         <f t="shared" si="0"/>
-        <v>125000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -963,21 +962,21 @@
         <v>20</v>
       </c>
       <c r="G17" s="4">
-        <f>1/2000*B17</f>
+        <f t="shared" ref="G17:G28" si="1">1/2000*B17</f>
         <v>0</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>3</v>
       </c>
       <c r="I17" s="3">
-        <f>1000/2000*B17</f>
+        <f t="shared" ref="I17:I28" si="2">1000/2000*B17</f>
         <v>0</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K17" s="4">
-        <f t="shared" ref="K17:K28" si="1">4096/1500</f>
+        <f t="shared" ref="K17:K28" si="3">4096/1500</f>
         <v>2.7306666666666666</v>
       </c>
       <c r="L17" s="1">
@@ -1001,21 +1000,21 @@
         <v>20</v>
       </c>
       <c r="G18" s="4">
-        <f>1/2000*B18</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I18" s="3">
-        <f>1000/2000*B18</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K18" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.7306666666666666</v>
       </c>
       <c r="L18" s="1">
@@ -1039,21 +1038,21 @@
         <v>20</v>
       </c>
       <c r="G19" s="4">
-        <f>1/2000*B19</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>3</v>
       </c>
       <c r="I19" s="3">
-        <f>1000/2000*B19</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K19" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.7306666666666666</v>
       </c>
       <c r="L19" s="1">
@@ -1077,21 +1076,21 @@
         <v>20</v>
       </c>
       <c r="G20" s="4">
-        <f>1/2000*B20</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I20" s="3">
-        <f>1000/2000*B20</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K20" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.7306666666666666</v>
       </c>
       <c r="L20" s="1">
@@ -1115,21 +1114,21 @@
         <v>24</v>
       </c>
       <c r="G21" s="4">
-        <f>1/2000*B21</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>3</v>
       </c>
       <c r="I21" s="3">
-        <f>1000/2000*B21</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K21" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.7306666666666666</v>
       </c>
       <c r="L21" s="1">
@@ -1156,21 +1155,21 @@
         <v>24</v>
       </c>
       <c r="G22" s="4">
-        <f>1/2000*B22</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I22" s="3">
-        <f>1000/2000*B22</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K22" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.7306666666666666</v>
       </c>
       <c r="L22" s="1">
@@ -1194,21 +1193,21 @@
         <v>24</v>
       </c>
       <c r="G23" s="4">
-        <f>1/2000*B23</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>3</v>
       </c>
       <c r="I23" s="3">
-        <f>1000/2000*B23</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K23" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.7306666666666666</v>
       </c>
       <c r="L23" s="1">
@@ -1232,21 +1231,21 @@
         <v>24</v>
       </c>
       <c r="G24" s="4">
-        <f>1/2000*B24</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I24" s="3">
-        <f>1000/2000*B24</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K24" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.7306666666666666</v>
       </c>
       <c r="L24" s="1">
@@ -1270,21 +1269,21 @@
         <v>20</v>
       </c>
       <c r="G25" s="4">
-        <f>1/2000*B25</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>25</v>
       </c>
       <c r="I25" s="3">
-        <f>1000/2000*B25</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K25" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.7306666666666666</v>
       </c>
       <c r="L25" s="1">
@@ -1308,21 +1307,21 @@
         <v>20</v>
       </c>
       <c r="G26" s="4">
-        <f>1/2000*B26</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>25</v>
       </c>
       <c r="I26" s="3">
-        <f>1000/2000*B26</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K26" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.7306666666666666</v>
       </c>
       <c r="L26" s="1">
@@ -1346,21 +1345,21 @@
         <v>24</v>
       </c>
       <c r="G27" s="4">
-        <f>1/2000*B27</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>25</v>
       </c>
       <c r="I27" s="3">
-        <f>1000/2000*B27</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K27" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.7306666666666666</v>
       </c>
       <c r="L27" s="1">
@@ -1384,21 +1383,21 @@
         <v>24</v>
       </c>
       <c r="G28" s="4">
-        <f>1/2000*B28</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>25</v>
       </c>
       <c r="I28" s="3">
-        <f>1000/2000*B28</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>21</v>
       </c>
       <c r="K28" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.7306666666666666</v>
       </c>
       <c r="L28" s="1">
@@ -1428,7 +1427,7 @@
       </c>
       <c r="B30" s="3">
         <f>E12</f>
-        <v>0</v>
+        <v>3906.25</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>54</v>
@@ -1438,7 +1437,7 @@
       </c>
       <c r="L30" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>25000</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
@@ -1477,21 +1476,21 @@
       </c>
       <c r="B32" s="3">
         <f>E38</f>
-        <v>1953.125</v>
+        <v>0</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E32" s="3">
         <f>50/100*B32</f>
-        <v>976.5625</v>
+        <v>0</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>29</v>
       </c>
       <c r="G32" s="4">
         <f>50/100*B32</f>
-        <v>976.5625</v>
+        <v>0</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>34</v>
@@ -1502,7 +1501,7 @@
       </c>
       <c r="L32" s="1">
         <f t="shared" si="0"/>
-        <v>9765.625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
@@ -1611,15 +1610,12 @@
       <c r="A38" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="1">
-        <v>1000000</v>
-      </c>
       <c r="D38" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E38" s="3">
         <f>1000/512000*B38</f>
-        <v>1953.125</v>
+        <v>0</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>36</v>
@@ -1629,12 +1625,15 @@
       <c r="A39" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="B39" s="1">
+        <v>1000000</v>
+      </c>
       <c r="D39" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E39" s="3">
         <f>1000/640000*B39</f>
-        <v>0</v>
+        <v>1562.5</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>36</v>
@@ -1670,7 +1669,7 @@
       </c>
       <c r="B47" s="1">
         <f>SUM(L:L)</f>
-        <v>384765.625</v>
+        <v>205000</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
@@ -1679,7 +1678,7 @@
       </c>
       <c r="B48" s="1">
         <f>B46-B47</f>
-        <v>615234.375</v>
+        <v>795000</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -1688,7 +1687,7 @@
       </c>
       <c r="B49" s="2">
         <f>B48/B46</f>
-        <v>0.615234375</v>
+        <v>0.79500000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>